<commit_message>
cleaned up file & project
</commit_message>
<xml_diff>
--- a/MovieRatingsTables.xlsx
+++ b/MovieRatingsTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Parker/Development_Projects/MovieRatings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A53B778-40FA-B646-8AA6-02367B00D36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D18CD6-9207-804A-BF7C-8B17442454A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{C99C7E33-DE92-EB4B-B53A-0CC77E47057E}"/>
   </bookViews>
@@ -34,7 +34,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+  <si>
+    <t>Parameters Tested</t>
+  </si>
   <si>
     <t>Optimizer</t>
   </si>
@@ -100,6 +103,18 @@
   </si>
   <si>
     <t>Validation Accuracy Table</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>rmsProp</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
   </si>
 </sst>
 </file>
@@ -258,7 +273,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -275,6 +290,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
@@ -592,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F328E58A-1349-1340-AFF2-B416673B78E3}">
-  <dimension ref="D5:K37"/>
+  <dimension ref="D5:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,245 +620,363 @@
     <col min="5" max="5" width="7.5" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:11" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:16" ht="24" x14ac:dyDescent="0.3">
       <c r="D5" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="4:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
       <c r="J7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D8" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="6"/>
       <c r="J8" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
       <c r="J9" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="P9" s="5">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="4:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D10" s="7"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="6"/>
       <c r="J10" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="M10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D11" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D12" s="7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="M12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D13" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="M13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D14" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="M14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D15" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D16" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="M16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D17" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="M17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D18" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D19" s="7"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="4:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D23" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D24" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D25" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D26" s="7"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D27" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D28" s="7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D29" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D30" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I30" s="5"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D31" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D32" s="7"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="6"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D33" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -850,7 +984,7 @@
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D34" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -864,7 +998,7 @@
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D36" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -872,7 +1006,7 @@
     </row>
     <row r="37" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D37" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>

</xml_diff>